<commit_message>
Updated testrun test file.
</commit_message>
<xml_diff>
--- a/tests/data/test_run.xlsx
+++ b/tests/data/test_run.xlsx
@@ -5,12 +5,15 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="tr####" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="ts####" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="tc####" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="tr0001" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="ts0001" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="tc0001" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="tc0002" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="asdf" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="827asaf" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="42">
   <si>
     <t xml:space="preserve">uuid:</t>
   </si>
@@ -42,12 +45,42 @@
     <t xml:space="preserve">test cases:</t>
   </si>
   <si>
+    <t xml:space="preserve">ts_uuid:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uuid-ts-01</t>
+  </si>
+  <si>
     <t xml:space="preserve">keywords:</t>
   </si>
   <si>
+    <t xml:space="preserve">test, test data, unkown results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tc0001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tc0002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">827asaf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tc_uuid:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uuid-tc-01</t>
+  </si>
+  <si>
     <t xml:space="preserve">title:</t>
   </si>
   <si>
+    <t xml:space="preserve">Test for test cases</t>
+  </si>
+  <si>
     <t xml:space="preserve">uuid</t>
   </si>
   <si>
@@ -58,6 +91,66 @@
   </si>
   <si>
     <t xml:space="preserve">parameter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selenium, click</t>
+  </si>
+  <si>
+    <t xml:space="preserve">para1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click answer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selenium, write</t>
+  </si>
+  <si>
+    <t xml:space="preserve">para2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Save answer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">para3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read answer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">para4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click next</t>
+  </si>
+  <si>
+    <t xml:space="preserve">para5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uuid-tc-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfj83jf-hf84-kg83-jhsh3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jf37gu-if83jf-8utgh4-gjr84</t>
   </si>
 </sst>
 </file>
@@ -72,6 +165,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -131,8 +225,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -159,29 +257,29 @@
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -201,25 +299,49 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -238,34 +360,476 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>7</v>
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>11</v>
+      <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated data model and created first version of conversion script from xlsx to json.
</commit_message>
<xml_diff>
--- a/tests/data/test_run.xlsx
+++ b/tests/data/test_run.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="tr0001" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,9 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="42">
-  <si>
-    <t xml:space="preserve">uuid:</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="44">
+  <si>
+    <t xml:space="preserve">tr_uuid:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tr100101</t>
   </si>
   <si>
     <t xml:space="preserve">start time:</t>
@@ -36,21 +39,36 @@
     <t xml:space="preserve">build:</t>
   </si>
   <si>
+    <t xml:space="preserve">V2.4</t>
+  </si>
+  <si>
     <t xml:space="preserve">end time:</t>
   </si>
   <si>
     <t xml:space="preserve">test suites:</t>
   </si>
   <si>
+    <t xml:space="preserve">uuid-ts-01</t>
+  </si>
+  <si>
     <t xml:space="preserve">test cases:</t>
   </si>
   <si>
+    <t xml:space="preserve">uuid-tc-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uuid-tc-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfj83jf-hf84-kg83-jhsh3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jf37gu-if83jf-8utgh4-gjr84</t>
+  </si>
+  <si>
     <t xml:space="preserve">ts_uuid:</t>
   </si>
   <si>
-    <t xml:space="preserve">uuid-ts-01</t>
-  </si>
-  <si>
     <t xml:space="preserve">keywords:</t>
   </si>
   <si>
@@ -72,9 +90,6 @@
     <t xml:space="preserve">tc_uuid:</t>
   </si>
   <si>
-    <t xml:space="preserve">uuid-tc-01</t>
-  </si>
-  <si>
     <t xml:space="preserve">title:</t>
   </si>
   <si>
@@ -142,15 +157,6 @@
   </si>
   <si>
     <t xml:space="preserve">para5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uuid-tc-02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dfj83jf-hf84-kg83-jhsh3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jf37gu-if83jf-8utgh4-gjr84</t>
   </si>
 </sst>
 </file>
@@ -251,36 +257,63 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D6" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -302,46 +335,46 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -363,107 +396,107 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -485,107 +518,107 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -607,107 +640,107 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -728,108 +761,108 @@
   </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated tests, test data, and fixed some bugs.
</commit_message>
<xml_diff>
--- a/tests/data/test_run.xlsx
+++ b/tests/data/test_run.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="tr0001" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="46">
   <si>
     <t xml:space="preserve">tr_uuid:</t>
   </si>
@@ -72,13 +72,19 @@
     <t xml:space="preserve">keywords:</t>
   </si>
   <si>
-    <t xml:space="preserve">test, test data, unkown results</t>
+    <t xml:space="preserve">test</t>
   </si>
   <si>
     <t xml:space="preserve">tc0001</t>
   </si>
   <si>
+    <t xml:space="preserve">test data</t>
+  </si>
+  <si>
     <t xml:space="preserve">tc0002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unkown results</t>
   </si>
   <si>
     <t xml:space="preserve">asdf</t>
@@ -259,17 +265,17 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -280,7 +286,7 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -334,11 +340,11 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -361,20 +367,26 @@
       <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="D2" s="0" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -399,104 +411,104 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -521,104 +533,104 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -643,104 +655,104 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -765,104 +777,104 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed duplicate step id detection.
</commit_message>
<xml_diff>
--- a/tests/data/test_run.xlsx
+++ b/tests/data/test_run.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="tr0001" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="51">
   <si>
     <t xml:space="preserve">tr_uuid:</t>
   </si>
@@ -163,6 +163,21 @@
   </si>
   <si>
     <t xml:space="preserve">para5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qewr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zxcv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qwer</t>
   </si>
 </sst>
 </file>
@@ -269,7 +284,7 @@
       <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -340,11 +355,11 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -367,7 +382,7 @@
       <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -375,7 +390,7 @@
       <c r="B3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -411,7 +426,7 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -527,13 +542,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -631,6 +646,20 @@
       </c>
       <c r="D7" s="1" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -649,13 +678,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -753,6 +782,20 @@
       </c>
       <c r="D7" s="1" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -771,13 +814,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -875,6 +918,20 @@
       </c>
       <c r="D7" s="1" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated conversion to create parameters object. Updated test file parsing to use new test file format.
</commit_message>
<xml_diff>
--- a/tests/data/test_run.xlsx
+++ b/tests/data/test_run.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="tr0001" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="60">
   <si>
     <t xml:space="preserve">tr_uuid:</t>
   </si>
@@ -99,24 +99,87 @@
     <t xml:space="preserve">title:</t>
   </si>
   <si>
+    <t xml:space="preserve">Tass Sample Run</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uuid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">action</t>
+  </si>
+  <si>
+    <t xml:space="preserve">locator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Launch test page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selenium,click</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click answer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selenium,write</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Save answer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read answer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click next</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">q12</t>
+  </si>
+  <si>
     <t xml:space="preserve">Test for test cases</t>
   </si>
   <si>
-    <t xml:space="preserve">uuid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">action</t>
-  </si>
-  <si>
     <t xml:space="preserve">parameter</t>
   </si>
   <si>
-    <t xml:space="preserve">q1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Open q1</t>
   </si>
   <si>
@@ -126,55 +189,19 @@
     <t xml:space="preserve">para1</t>
   </si>
   <si>
-    <t xml:space="preserve">q2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Click answer</t>
-  </si>
-  <si>
     <t xml:space="preserve">selenium, write</t>
   </si>
   <si>
     <t xml:space="preserve">para2</t>
   </si>
   <si>
-    <t xml:space="preserve">q3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Save answer</t>
-  </si>
-  <si>
     <t xml:space="preserve">para3</t>
   </si>
   <si>
-    <t xml:space="preserve">q4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Read answer</t>
-  </si>
-  <si>
     <t xml:space="preserve">para4</t>
   </si>
   <si>
-    <t xml:space="preserve">q5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Click next</t>
-  </si>
-  <si>
     <t xml:space="preserve">para5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">q7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">qewr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">zxcv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">q6</t>
   </si>
   <si>
     <t xml:space="preserve">qwer</t>
@@ -281,10 +308,10 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -359,7 +386,7 @@
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -420,13 +447,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -455,20 +482,21 @@
       <c r="D2" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="E2" s="0" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -480,50 +508,77 @@
       <c r="C4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>39</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="D5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="D6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="1" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="1" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -542,13 +597,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -561,7 +616,7 @@
         <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -575,92 +630,38 @@
         <v>27</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>48</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -684,7 +685,7 @@
       <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -697,7 +698,7 @@
         <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -711,21 +712,21 @@
         <v>27</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -736,57 +737,57 @@
         <v>34</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>20</v>
@@ -820,7 +821,7 @@
       <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -833,7 +834,7 @@
         <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -847,21 +848,21 @@
         <v>27</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -872,57 +873,57 @@
         <v>34</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>20</v>
@@ -931,7 +932,7 @@
         <v>20</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>